<commit_message>
divide yrs of school by 25 yrs
</commit_message>
<xml_diff>
--- a/data/Mincer_YrsSchool.xlsx
+++ b/data/Mincer_YrsSchool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Documents\GitHub\teachers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0FBC47-6ACD-47A5-BC6E-A957562ABD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D76F3C-5E02-4E6C-82CC-F2C5AE234135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{3531A8FF-D0DF-4403-A910-B6CFC06880B8}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
   <si>
     <t>ln (hourly wage in $1999)=const+b1*school+b2*age+b3*age^2+e</t>
   </si>
@@ -138,6 +138,9 @@
   <si>
     <t>Min 9, max 17 years of school</t>
   </si>
+  <si>
+    <t>As in Hsieh et al, we divide yrs of schooling by 25</t>
+  </si>
 </sst>
 </file>
 
@@ -181,14 +184,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,19 +532,19 @@
       <c r="B4">
         <v>1960</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>1970</v>
       </c>
       <c r="D4">
         <v>1980</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>1990</v>
       </c>
       <c r="F4">
         <v>2000</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>2010</v>
       </c>
     </row>
@@ -551,29 +555,29 @@
       <c r="B5" s="1">
         <v>4.4667600000000002E-2</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>5.3321199999999999E-2</v>
       </c>
       <c r="D5" s="1">
         <v>4.90593E-2</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>8.25322E-2</v>
       </c>
       <c r="F5" s="1">
         <v>8.9569899999999994E-2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>0.10256319999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
-      <c r="C6" s="4"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -582,19 +586,19 @@
       <c r="B7" s="1">
         <v>3.9692031906802254E-2</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>4.7471048681422184E-2</v>
       </c>
       <c r="D7" s="1">
         <v>4.5976864536856045E-2</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>7.7059687667519472E-2</v>
       </c>
       <c r="F7" s="1">
         <v>8.2138246754080921E-2</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>9.6556296030251135E-2</v>
       </c>
     </row>
@@ -605,19 +609,19 @@
       <c r="B8" s="1">
         <v>3.7630682204947377E-2</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>4.409366478932937E-2</v>
       </c>
       <c r="D8" s="1">
         <v>4.0162686188585865E-2</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>6.8209358946771853E-2</v>
       </c>
       <c r="F8" s="1">
         <v>7.2688045151711525E-2</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>8.3074437174163407E-2</v>
       </c>
     </row>
@@ -628,19 +632,19 @@
       <c r="B9" s="1">
         <v>4.7699135102262057E-2</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>5.8395997008662423E-2</v>
       </c>
       <c r="D9" s="1">
         <v>5.6754782376008638E-2</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>8.9878162009358498E-2</v>
       </c>
       <c r="F9" s="1">
         <v>9.4996393622356748E-2</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>0.11229458258696567</v>
       </c>
     </row>
@@ -666,30 +670,30 @@
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="4">
         <v>1960</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4">
         <v>1970</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4">
         <v>1980</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4">
         <v>1990</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4">
         <v>2000</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4">
         <v>2010</v>
       </c>
-      <c r="M1" s="2"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1568,30 +1572,30 @@
       <c r="A25" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="4">
         <v>1960</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4">
         <v>1970</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2">
+      <c r="E25" s="4"/>
+      <c r="F25" s="4">
         <v>1980</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4">
         <v>1990</v>
       </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2">
+      <c r="I25" s="4"/>
+      <c r="J25" s="4">
         <v>2000</v>
       </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2">
+      <c r="K25" s="4"/>
+      <c r="L25" s="4">
         <v>2010</v>
       </c>
-      <c r="M25" s="2"/>
+      <c r="M25" s="4"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -2516,1043 +2520,2136 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C962E32-AF3E-4EA7-84B5-4BB144D082EC}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="7.140625" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="7.140625" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
       <c r="B4">
         <v>1960</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>1970</v>
       </c>
       <c r="D4">
         <v>1980</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>1990</v>
       </c>
       <c r="F4">
         <v>2000</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>2013</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>1960</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1970</v>
+      </c>
+      <c r="K4">
+        <v>1980</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1990</v>
+      </c>
+      <c r="M4">
+        <v>2000</v>
+      </c>
+      <c r="N4" s="2">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>12.22824</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>12.78478</v>
       </c>
       <c r="D5" s="1">
         <v>13.00365</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>12.487730000000001</v>
       </c>
       <c r="F5" s="1">
         <v>12.44459</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>12.493589999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5" s="1">
+        <f>B5/25</f>
+        <v>0.4891296</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" ref="J5:N5" si="0">C5/25</f>
+        <v>0.51139119999999993</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.520146</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49950920000000004</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.49778359999999999</v>
+      </c>
+      <c r="N5" s="3">
+        <f t="shared" si="0"/>
+        <v>0.49974359999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>13.29659</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>13.651450000000001</v>
       </c>
       <c r="D6" s="1">
         <v>14.68768</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>14.24555</v>
       </c>
       <c r="F6" s="1">
         <v>14.48765</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>14.81123</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="1">
+        <f t="shared" ref="I6:I25" si="1">B6/25</f>
+        <v>0.53186359999999999</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" ref="J6:J25" si="2">C6/25</f>
+        <v>0.54605800000000004</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" ref="K6:K25" si="3">D6/25</f>
+        <v>0.58750720000000001</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" ref="L6:L25" si="4">E6/25</f>
+        <v>0.56982199999999994</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" ref="M6:M25" si="5">F6/25</f>
+        <v>0.57950599999999997</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" ref="N6:N25" si="6">G6/25</f>
+        <v>0.59244920000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="1">
         <v>14.3391</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>14.6595</v>
       </c>
       <c r="D7" s="1">
         <v>15.39391</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>15.181319999999999</v>
       </c>
       <c r="F7" s="1">
         <v>15.280860000000001</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>15.61294</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.57356399999999996</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.58638000000000001</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="3"/>
+        <v>0.61575639999999998</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="4"/>
+        <v>0.60725279999999993</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="5"/>
+        <v>0.61123440000000007</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="6"/>
+        <v>0.62451760000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="1">
         <v>15.272959999999999</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>15.308619999999999</v>
       </c>
       <c r="D8" s="1">
         <v>15.61407</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>15.522880000000001</v>
       </c>
       <c r="F8" s="1">
         <v>15.21969</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>15.401999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>0.61091839999999997</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.61234480000000002</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="3"/>
+        <v>0.62456279999999997</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="4"/>
+        <v>0.6209152</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="5"/>
+        <v>0.60878759999999998</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="6"/>
+        <v>0.61607999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1">
         <v>15.261189999999999</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>15.12725</v>
       </c>
       <c r="D9" s="1">
         <v>15.494859999999999</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>15.06687</v>
       </c>
       <c r="F9" s="1">
         <v>15.20979</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>15.42985</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="1">
+        <f t="shared" si="1"/>
+        <v>0.61044759999999998</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.60509000000000002</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="3"/>
+        <v>0.61979439999999997</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="4"/>
+        <v>0.60267479999999995</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="5"/>
+        <v>0.60839160000000003</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="6"/>
+        <v>0.61719400000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="1">
         <v>16.883929999999999</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>16.870280000000001</v>
       </c>
       <c r="D10" s="1">
         <v>16.913119999999999</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>16.93984</v>
       </c>
       <c r="F10" s="1">
         <v>16.943729999999999</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>16.952780000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <f t="shared" si="1"/>
+        <v>0.67535719999999999</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.67481120000000006</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="3"/>
+        <v>0.67652479999999993</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="4"/>
+        <v>0.67759360000000002</v>
+      </c>
+      <c r="M10" s="1">
+        <f t="shared" si="5"/>
+        <v>0.67774919999999994</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="6"/>
+        <v>0.67811120000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="1">
         <v>14.15227</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>14.4328</v>
       </c>
       <c r="D11" s="1">
         <v>14.876390000000001</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>14.244260000000001</v>
       </c>
       <c r="F11" s="1">
         <v>14.383039999999999</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>14.53445</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>0.56609080000000001</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.57731200000000005</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="3"/>
+        <v>0.59505560000000002</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="4"/>
+        <v>0.56977040000000001</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="5"/>
+        <v>0.57532159999999999</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="6"/>
+        <v>0.58137799999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="1">
         <v>16.815370000000001</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>16.81757</v>
       </c>
       <c r="D12" s="1">
         <v>16.657050000000002</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>16.419750000000001</v>
       </c>
       <c r="F12" s="1">
         <v>16.346879999999999</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>16.591259999999998</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>0.67261480000000007</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="2"/>
+        <v>0.67270280000000005</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="3"/>
+        <v>0.66628200000000004</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="4"/>
+        <v>0.65678999999999998</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="5"/>
+        <v>0.65387519999999999</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="6"/>
+        <v>0.66365039999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="1">
         <v>16.11429</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>16.324729999999999</v>
       </c>
       <c r="D13" s="1">
         <v>16.046230000000001</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>15.276439999999999</v>
       </c>
       <c r="F13" s="1">
         <v>14.88795</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>15.22687</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>0.64457160000000002</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="2"/>
+        <v>0.65298919999999994</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="3"/>
+        <v>0.64184920000000001</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="4"/>
+        <v>0.61105759999999998</v>
+      </c>
+      <c r="M13" s="1">
+        <f t="shared" si="5"/>
+        <v>0.59551799999999999</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="6"/>
+        <v>0.60907480000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="1">
         <v>13.462120000000001</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>13.72724</v>
       </c>
       <c r="D14" s="1">
         <v>14.372540000000001</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>14.18816</v>
       </c>
       <c r="F14" s="1">
         <v>14.61556</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>14.91309</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.53848479999999999</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="2"/>
+        <v>0.54908959999999996</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="3"/>
+        <v>0.57490160000000001</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="4"/>
+        <v>0.56752639999999999</v>
+      </c>
+      <c r="M14" s="1">
+        <f t="shared" si="5"/>
+        <v>0.58462239999999999</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="6"/>
+        <v>0.59652360000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>13.285159999999999</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>13.485239999999999</v>
       </c>
       <c r="D15" s="1">
         <v>14.170669999999999</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>13.75624</v>
       </c>
       <c r="F15" s="1">
         <v>13.74921</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>13.90218</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.53140639999999995</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="2"/>
+        <v>0.53940959999999993</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="3"/>
+        <v>0.56682679999999996</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="4"/>
+        <v>0.55024960000000001</v>
+      </c>
+      <c r="M15" s="1">
+        <f t="shared" si="5"/>
+        <v>0.54996840000000002</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="6"/>
+        <v>0.5560872</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>12.64223</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>12.951180000000001</v>
       </c>
       <c r="D16" s="1">
         <v>13.707789999999999</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>13.370139999999999</v>
       </c>
       <c r="F16" s="1">
         <v>13.31696</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>13.578609999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.50568919999999995</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="2"/>
+        <v>0.51804720000000004</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="3"/>
+        <v>0.54831160000000001</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="4"/>
+        <v>0.53480559999999999</v>
+      </c>
+      <c r="M16" s="1">
+        <f t="shared" si="5"/>
+        <v>0.5326784</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="6"/>
+        <v>0.54314439999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="1">
         <v>11.90493</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>12.37771</v>
       </c>
       <c r="D17" s="1">
         <v>13.517110000000001</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>13.233890000000001</v>
       </c>
       <c r="F17" s="1">
         <v>13.36159</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>13.644130000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.47619719999999999</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="2"/>
+        <v>0.4951084</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="3"/>
+        <v>0.54068440000000006</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" si="4"/>
+        <v>0.52935560000000004</v>
+      </c>
+      <c r="M17" s="1">
+        <f t="shared" si="5"/>
+        <v>0.53446360000000004</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="6"/>
+        <v>0.54576520000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="1">
         <v>11.224679999999999</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>11.66821</v>
       </c>
       <c r="D18" s="1">
         <v>12.67615</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>12.468970000000001</v>
       </c>
       <c r="F18" s="1">
         <v>12.57119</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>12.77087</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="1">
+        <f t="shared" si="1"/>
+        <v>0.44898719999999998</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="2"/>
+        <v>0.46672839999999999</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="3"/>
+        <v>0.507046</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" si="4"/>
+        <v>0.4987588</v>
+      </c>
+      <c r="M18" s="1">
+        <f t="shared" si="5"/>
+        <v>0.50284759999999995</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="6"/>
+        <v>0.51083480000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="1">
         <v>11.65202</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>11.94721</v>
       </c>
       <c r="D19" s="1">
         <v>12.789389999999999</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>12.34801</v>
       </c>
       <c r="F19" s="1">
         <v>12.330080000000001</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>12.504379999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.46608080000000002</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="2"/>
+        <v>0.47788839999999999</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="3"/>
+        <v>0.51157560000000002</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="4"/>
+        <v>0.49392040000000004</v>
+      </c>
+      <c r="M19" s="1">
+        <f t="shared" si="5"/>
+        <v>0.49320320000000001</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="6"/>
+        <v>0.50017519999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="1">
         <v>11.466670000000001</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>11.71613</v>
       </c>
       <c r="D20" s="1">
         <v>12.498699999999999</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>12.337680000000001</v>
       </c>
       <c r="F20" s="1">
         <v>12.27882</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>12.475110000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="1">
+        <f t="shared" si="1"/>
+        <v>0.45866680000000004</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="2"/>
+        <v>0.46864519999999998</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="3"/>
+        <v>0.499948</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="4"/>
+        <v>0.49350720000000003</v>
+      </c>
+      <c r="M20" s="1">
+        <f t="shared" si="5"/>
+        <v>0.4911528</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="6"/>
+        <v>0.49900440000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="1">
         <v>11.761060000000001</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>12.058350000000001</v>
       </c>
       <c r="D21" s="1">
         <v>12.82138</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>12.507300000000001</v>
       </c>
       <c r="F21" s="1">
         <v>12.48377</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>12.675599999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="1">
+        <f t="shared" si="1"/>
+        <v>0.47044240000000004</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.48233400000000004</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="3"/>
+        <v>0.51285519999999996</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="4"/>
+        <v>0.50029200000000007</v>
+      </c>
+      <c r="M21" s="1">
+        <f t="shared" si="5"/>
+        <v>0.49935079999999998</v>
+      </c>
+      <c r="N21" s="3">
+        <f t="shared" si="6"/>
+        <v>0.50702399999999992</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="1">
         <v>11.382110000000001</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>11.559900000000001</v>
       </c>
       <c r="D22" s="1">
         <v>12.22175</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>12.211819999999999</v>
       </c>
       <c r="F22" s="1">
         <v>12.157780000000001</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>12.400639999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="1">
+        <f t="shared" si="1"/>
+        <v>0.45528440000000003</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="2"/>
+        <v>0.46239600000000003</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="3"/>
+        <v>0.48887000000000003</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="4"/>
+        <v>0.48847279999999998</v>
+      </c>
+      <c r="M22" s="1">
+        <f t="shared" si="5"/>
+        <v>0.48631120000000005</v>
+      </c>
+      <c r="N22" s="3">
+        <f t="shared" si="6"/>
+        <v>0.49602559999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>11.37574</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>11.6472</v>
       </c>
       <c r="D23" s="1">
         <v>12.263310000000001</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>12.23624</v>
       </c>
       <c r="F23" s="1">
         <v>12.22404</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>12.418010000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" s="1">
+        <f t="shared" si="1"/>
+        <v>0.45502960000000003</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="2"/>
+        <v>0.46588799999999997</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="3"/>
+        <v>0.49053240000000004</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.48944960000000004</v>
+      </c>
+      <c r="M23" s="1">
+        <f t="shared" si="5"/>
+        <v>0.4889616</v>
+      </c>
+      <c r="N23" s="3">
+        <f t="shared" si="6"/>
+        <v>0.49672040000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>11.10716</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>11.453849999999999</v>
       </c>
       <c r="D24" s="1">
         <v>12.19993</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>12.16836</v>
       </c>
       <c r="F24" s="1">
         <v>12.195460000000001</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>12.41521</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="1">
+        <f t="shared" si="1"/>
+        <v>0.44428640000000003</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.45815399999999995</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="3"/>
+        <v>0.48799720000000002</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="4"/>
+        <v>0.48673440000000001</v>
+      </c>
+      <c r="M24" s="1">
+        <f t="shared" si="5"/>
+        <v>0.48781840000000004</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="6"/>
+        <v>0.49660840000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="1">
         <v>16.223510000000001</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>16.24015</v>
       </c>
       <c r="D25" s="1">
         <v>16.295839999999998</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>15.71311</v>
       </c>
       <c r="F25" s="1">
         <v>15.958920000000001</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <v>16.040500000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="1">
+        <f t="shared" si="1"/>
+        <v>0.64894040000000008</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="2"/>
+        <v>0.64960600000000002</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="3"/>
+        <v>0.6518335999999999</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="4"/>
+        <v>0.62852439999999998</v>
+      </c>
+      <c r="M25" s="1">
+        <f t="shared" si="5"/>
+        <v>0.63835680000000006</v>
+      </c>
+      <c r="N25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.64162000000000008</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
       <c r="B27">
         <v>1960</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>1970</v>
       </c>
       <c r="D27">
         <v>1980</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>1990</v>
       </c>
       <c r="F27">
         <v>2000</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>2013</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>1960</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1970</v>
+      </c>
+      <c r="K27">
+        <v>1980</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1990</v>
+      </c>
+      <c r="M27">
+        <v>2000</v>
+      </c>
+      <c r="N27" s="2">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="1">
         <v>11.97016</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>12.288</v>
       </c>
       <c r="D28" s="1">
         <v>12.69694</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="3">
         <v>12.66155</v>
       </c>
       <c r="F28" s="1">
         <v>12.864599999999999</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>13.20467</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="1">
+        <f>B28/25</f>
+        <v>0.47880640000000002</v>
+      </c>
+      <c r="J28" s="3">
+        <f t="shared" ref="J28:J48" si="7">C28/25</f>
+        <v>0.49152000000000001</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" ref="K28:K48" si="8">D28/25</f>
+        <v>0.50787760000000004</v>
+      </c>
+      <c r="L28" s="3">
+        <f t="shared" ref="L28:L48" si="9">E28/25</f>
+        <v>0.50646199999999997</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" ref="M28:M48" si="10">F28/25</f>
+        <v>0.51458399999999993</v>
+      </c>
+      <c r="N28" s="3">
+        <f t="shared" ref="N28:N48" si="11">G28/25</f>
+        <v>0.52818679999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="1">
         <v>12.488910000000001</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>12.96879</v>
       </c>
       <c r="D29" s="1">
         <v>14.067880000000001</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>14.025980000000001</v>
       </c>
       <c r="F29" s="1">
         <v>14.51587</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>15.076280000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="1">
+        <f t="shared" ref="I29:I48" si="12">B29/25</f>
+        <v>0.49955640000000001</v>
+      </c>
+      <c r="J29" s="3">
+        <f t="shared" si="7"/>
+        <v>0.51875159999999998</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="8"/>
+        <v>0.56271519999999997</v>
+      </c>
+      <c r="L29" s="3">
+        <f t="shared" si="9"/>
+        <v>0.56103920000000007</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" si="10"/>
+        <v>0.58063480000000001</v>
+      </c>
+      <c r="N29" s="3">
+        <f t="shared" si="11"/>
+        <v>0.60305120000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
       <c r="B30" s="1">
         <v>12.785349999999999</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>13.110989999999999</v>
       </c>
       <c r="D30" s="1">
         <v>14.261189999999999</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="3">
         <v>14.51066</v>
       </c>
       <c r="F30" s="1">
         <v>14.81659</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>15.40014</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="1">
+        <f t="shared" si="12"/>
+        <v>0.51141399999999992</v>
+      </c>
+      <c r="J30" s="3">
+        <f t="shared" si="7"/>
+        <v>0.52443960000000001</v>
+      </c>
+      <c r="K30" s="1">
+        <f t="shared" si="8"/>
+        <v>0.57044759999999994</v>
+      </c>
+      <c r="L30" s="3">
+        <f t="shared" si="9"/>
+        <v>0.58042640000000001</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" si="10"/>
+        <v>0.59266359999999996</v>
+      </c>
+      <c r="N30" s="3">
+        <f t="shared" si="11"/>
+        <v>0.61600560000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="1">
         <v>14.755000000000001</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>14.79725</v>
       </c>
       <c r="D31" s="1">
         <v>15.071569999999999</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="3">
         <v>15.32039</v>
       </c>
       <c r="F31" s="1">
         <v>15.227510000000001</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <v>15.661949999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="1">
+        <f t="shared" si="12"/>
+        <v>0.59020000000000006</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="shared" si="7"/>
+        <v>0.59189000000000003</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="8"/>
+        <v>0.60286280000000003</v>
+      </c>
+      <c r="L31" s="3">
+        <f t="shared" si="9"/>
+        <v>0.61281560000000002</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="10"/>
+        <v>0.60910039999999999</v>
+      </c>
+      <c r="N31" s="3">
+        <f t="shared" si="11"/>
+        <v>0.62647799999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="1">
         <v>14.95237</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>14.94534</v>
       </c>
       <c r="D32" s="1">
         <v>15.32455</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <v>15.087949999999999</v>
       </c>
       <c r="F32" s="1">
         <v>15.380089999999999</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <v>15.71597</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="1">
+        <f t="shared" si="12"/>
+        <v>0.59809480000000004</v>
+      </c>
+      <c r="J32" s="3">
+        <f t="shared" si="7"/>
+        <v>0.59781359999999995</v>
+      </c>
+      <c r="K32" s="1">
+        <f t="shared" si="8"/>
+        <v>0.61298200000000003</v>
+      </c>
+      <c r="L32" s="3">
+        <f t="shared" si="9"/>
+        <v>0.603518</v>
+      </c>
+      <c r="M32" s="1">
+        <f t="shared" si="10"/>
+        <v>0.61520359999999996</v>
+      </c>
+      <c r="N32" s="3">
+        <f t="shared" si="11"/>
+        <v>0.62863880000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
       <c r="B33" s="1">
         <v>16.282959999999999</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>16.36232</v>
       </c>
       <c r="D33" s="1">
         <v>16.536010000000001</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <v>16.849979999999999</v>
       </c>
       <c r="F33" s="1">
         <v>16.92043</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <v>16.92653</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="1">
+        <f t="shared" si="12"/>
+        <v>0.65131839999999996</v>
+      </c>
+      <c r="J33" s="3">
+        <f t="shared" si="7"/>
+        <v>0.65449279999999999</v>
+      </c>
+      <c r="K33" s="1">
+        <f t="shared" si="8"/>
+        <v>0.66144040000000004</v>
+      </c>
+      <c r="L33" s="3">
+        <f t="shared" si="9"/>
+        <v>0.67399919999999991</v>
+      </c>
+      <c r="M33" s="1">
+        <f t="shared" si="10"/>
+        <v>0.67681720000000001</v>
+      </c>
+      <c r="N33" s="3">
+        <f t="shared" si="11"/>
+        <v>0.67706120000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
       <c r="B34" s="1">
         <v>13.20942</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>13.11894</v>
       </c>
       <c r="D34" s="1">
         <v>14.104179999999999</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="3">
         <v>14.041460000000001</v>
       </c>
       <c r="F34" s="1">
         <v>13.96428</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <v>14.269030000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="1">
+        <f t="shared" si="12"/>
+        <v>0.52837679999999998</v>
+      </c>
+      <c r="J34" s="3">
+        <f t="shared" si="7"/>
+        <v>0.52475760000000005</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" si="8"/>
+        <v>0.56416719999999998</v>
+      </c>
+      <c r="L34" s="3">
+        <f t="shared" si="9"/>
+        <v>0.5616584</v>
+      </c>
+      <c r="M34" s="1">
+        <f t="shared" si="10"/>
+        <v>0.55857120000000005</v>
+      </c>
+      <c r="N34" s="3">
+        <f t="shared" si="11"/>
+        <v>0.57076120000000008</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>15</v>
       </c>
       <c r="B35" s="1">
         <v>16.58042</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>16.540980000000001</v>
       </c>
       <c r="D35" s="1">
         <v>16.513729999999999</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>16.27664</v>
       </c>
       <c r="F35" s="1">
         <v>16.294589999999999</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="3">
         <v>16.588840000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" s="1">
+        <f t="shared" si="12"/>
+        <v>0.66321680000000005</v>
+      </c>
+      <c r="J35" s="3">
+        <f t="shared" si="7"/>
+        <v>0.66163920000000009</v>
+      </c>
+      <c r="K35" s="1">
+        <f t="shared" si="8"/>
+        <v>0.66054919999999995</v>
+      </c>
+      <c r="L35" s="3">
+        <f t="shared" si="9"/>
+        <v>0.65106560000000002</v>
+      </c>
+      <c r="M35" s="1">
+        <f t="shared" si="10"/>
+        <v>0.65178360000000002</v>
+      </c>
+      <c r="N35" s="3">
+        <f t="shared" si="11"/>
+        <v>0.66355360000000008</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="1">
         <v>15.28998</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>14.394640000000001</v>
       </c>
       <c r="D36" s="1">
         <v>14.99117</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>13.8043</v>
       </c>
       <c r="F36" s="1">
         <v>14.247629999999999</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <v>15.15333</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" s="1">
+        <f t="shared" si="12"/>
+        <v>0.61159920000000001</v>
+      </c>
+      <c r="J36" s="3">
+        <f t="shared" si="7"/>
+        <v>0.57578560000000001</v>
+      </c>
+      <c r="K36" s="1">
+        <f t="shared" si="8"/>
+        <v>0.59964680000000004</v>
+      </c>
+      <c r="L36" s="3">
+        <f t="shared" si="9"/>
+        <v>0.552172</v>
+      </c>
+      <c r="M36" s="1">
+        <f t="shared" si="10"/>
+        <v>0.5699052</v>
+      </c>
+      <c r="N36" s="3">
+        <f t="shared" si="11"/>
+        <v>0.60613320000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
       <c r="B37" s="1">
         <v>13.198600000000001</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>13.6671</v>
       </c>
       <c r="D37" s="1">
         <v>13.989570000000001</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>14.085599999999999</v>
       </c>
       <c r="F37" s="1">
         <v>14.18314</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="3">
         <v>14.43698</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" s="1">
+        <f t="shared" si="12"/>
+        <v>0.52794400000000008</v>
+      </c>
+      <c r="J37" s="3">
+        <f t="shared" si="7"/>
+        <v>0.54668399999999995</v>
+      </c>
+      <c r="K37" s="1">
+        <f t="shared" si="8"/>
+        <v>0.55958280000000005</v>
+      </c>
+      <c r="L37" s="3">
+        <f t="shared" si="9"/>
+        <v>0.56342399999999992</v>
+      </c>
+      <c r="M37" s="1">
+        <f t="shared" si="10"/>
+        <v>0.56732559999999999</v>
+      </c>
+      <c r="N37" s="3">
+        <f t="shared" si="11"/>
+        <v>0.57747919999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="1">
         <v>11.57583</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <v>11.95613</v>
       </c>
       <c r="D38" s="1">
         <v>13.0396</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>13.22565</v>
       </c>
       <c r="F38" s="1">
         <v>13.25614</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="3">
         <v>13.60238</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38" s="1">
+        <f t="shared" si="12"/>
+        <v>0.46303319999999998</v>
+      </c>
+      <c r="J38" s="3">
+        <f t="shared" si="7"/>
+        <v>0.47824519999999998</v>
+      </c>
+      <c r="K38" s="1">
+        <f t="shared" si="8"/>
+        <v>0.52158400000000005</v>
+      </c>
+      <c r="L38" s="3">
+        <f t="shared" si="9"/>
+        <v>0.529026</v>
+      </c>
+      <c r="M38" s="1">
+        <f t="shared" si="10"/>
+        <v>0.53024559999999998</v>
+      </c>
+      <c r="N38" s="3">
+        <f t="shared" si="11"/>
+        <v>0.5440952</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
       <c r="B39" s="1">
         <v>12.20285</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="3">
         <v>12.405340000000001</v>
       </c>
       <c r="D39" s="1">
         <v>12.931319999999999</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="3">
         <v>13.05728</v>
       </c>
       <c r="F39" s="1">
         <v>13.1401</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="3">
         <v>13.635949999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39" s="1">
+        <f t="shared" si="12"/>
+        <v>0.48811399999999999</v>
+      </c>
+      <c r="J39" s="3">
+        <f t="shared" si="7"/>
+        <v>0.49621360000000003</v>
+      </c>
+      <c r="K39" s="1">
+        <f t="shared" si="8"/>
+        <v>0.51725279999999996</v>
+      </c>
+      <c r="L39" s="3">
+        <f t="shared" si="9"/>
+        <v>0.52229120000000007</v>
+      </c>
+      <c r="M39" s="1">
+        <f t="shared" si="10"/>
+        <v>0.52560399999999996</v>
+      </c>
+      <c r="N39" s="3">
+        <f t="shared" si="11"/>
+        <v>0.54543799999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>20</v>
       </c>
       <c r="B40" s="1">
         <v>12.06306</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="3">
         <v>12.014810000000001</v>
       </c>
       <c r="D40" s="1">
         <v>13.232200000000001</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>13.327199999999999</v>
       </c>
       <c r="F40" s="1">
         <v>13.35144</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="3">
         <v>13.90095</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40" s="1">
+        <f t="shared" si="12"/>
+        <v>0.48252240000000002</v>
+      </c>
+      <c r="J40" s="3">
+        <f t="shared" si="7"/>
+        <v>0.48059240000000003</v>
+      </c>
+      <c r="K40" s="1">
+        <f t="shared" si="8"/>
+        <v>0.52928799999999998</v>
+      </c>
+      <c r="L40" s="3">
+        <f t="shared" si="9"/>
+        <v>0.53308800000000001</v>
+      </c>
+      <c r="M40" s="1">
+        <f t="shared" si="10"/>
+        <v>0.53405760000000002</v>
+      </c>
+      <c r="N40" s="3">
+        <f t="shared" si="11"/>
+        <v>0.55603800000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
       </c>
       <c r="B41" s="1">
         <v>11.109830000000001</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="3">
         <v>11.385070000000001</v>
       </c>
       <c r="D41" s="1">
         <v>12.2544</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="3">
         <v>12.41606</v>
       </c>
       <c r="F41" s="1">
         <v>12.56499</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="3">
         <v>12.91358</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41" s="1">
+        <f t="shared" si="12"/>
+        <v>0.44439320000000004</v>
+      </c>
+      <c r="J41" s="3">
+        <f t="shared" si="7"/>
+        <v>0.45540280000000005</v>
+      </c>
+      <c r="K41" s="1">
+        <f t="shared" si="8"/>
+        <v>0.490176</v>
+      </c>
+      <c r="L41" s="3">
+        <f t="shared" si="9"/>
+        <v>0.49664239999999998</v>
+      </c>
+      <c r="M41" s="1">
+        <f t="shared" si="10"/>
+        <v>0.50259960000000004</v>
+      </c>
+      <c r="N41" s="3">
+        <f t="shared" si="11"/>
+        <v>0.51654319999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
       <c r="B42" s="1">
         <v>11.431940000000001</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="3">
         <v>11.698259999999999</v>
       </c>
       <c r="D42" s="1">
         <v>12.72865</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="3">
         <v>12.67414</v>
       </c>
       <c r="F42" s="1">
         <v>12.62147</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="3">
         <v>13.16794</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42" s="1">
+        <f t="shared" si="12"/>
+        <v>0.45727760000000006</v>
+      </c>
+      <c r="J42" s="3">
+        <f t="shared" si="7"/>
+        <v>0.46793039999999997</v>
+      </c>
+      <c r="K42" s="1">
+        <f t="shared" si="8"/>
+        <v>0.50914599999999999</v>
+      </c>
+      <c r="L42" s="3">
+        <f t="shared" si="9"/>
+        <v>0.50696560000000002</v>
+      </c>
+      <c r="M42" s="1">
+        <f t="shared" si="10"/>
+        <v>0.50485880000000005</v>
+      </c>
+      <c r="N42" s="3">
+        <f t="shared" si="11"/>
+        <v>0.52671760000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="1">
         <v>11.5374</v>
       </c>
-      <c r="C43" s="4">
+      <c r="C43" s="3">
         <v>11.541510000000001</v>
       </c>
       <c r="D43" s="1">
         <v>12.569039999999999</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="3">
         <v>12.74536</v>
       </c>
       <c r="F43" s="1">
         <v>12.71677</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="3">
         <v>13.20481</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43" s="1">
+        <f t="shared" si="12"/>
+        <v>0.46149600000000002</v>
+      </c>
+      <c r="J43" s="3">
+        <f t="shared" si="7"/>
+        <v>0.46166040000000003</v>
+      </c>
+      <c r="K43" s="1">
+        <f t="shared" si="8"/>
+        <v>0.50276159999999992</v>
+      </c>
+      <c r="L43" s="3">
+        <f t="shared" si="9"/>
+        <v>0.5098144</v>
+      </c>
+      <c r="M43" s="1">
+        <f t="shared" si="10"/>
+        <v>0.50867079999999998</v>
+      </c>
+      <c r="N43" s="3">
+        <f t="shared" si="11"/>
+        <v>0.52819240000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>24</v>
       </c>
       <c r="B44" s="1">
         <v>11.380599999999999</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="3">
         <v>11.61337</v>
       </c>
       <c r="D44" s="1">
         <v>12.48743</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="3">
         <v>12.521430000000001</v>
       </c>
       <c r="F44" s="1">
         <v>12.60385</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="3">
         <v>13.01999</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44" s="1">
+        <f t="shared" si="12"/>
+        <v>0.45522399999999996</v>
+      </c>
+      <c r="J44" s="3">
+        <f t="shared" si="7"/>
+        <v>0.46453479999999997</v>
+      </c>
+      <c r="K44" s="1">
+        <f t="shared" si="8"/>
+        <v>0.49949719999999997</v>
+      </c>
+      <c r="L44" s="3">
+        <f t="shared" si="9"/>
+        <v>0.5008572</v>
+      </c>
+      <c r="M44" s="1">
+        <f t="shared" si="10"/>
+        <v>0.50415399999999999</v>
+      </c>
+      <c r="N44" s="3">
+        <f t="shared" si="11"/>
+        <v>0.52079960000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>25</v>
       </c>
       <c r="B45" s="1">
         <v>10.9176</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C45" s="3">
         <v>11.14508</v>
       </c>
       <c r="D45" s="1">
         <v>11.7037</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="3">
         <v>12.016970000000001</v>
       </c>
       <c r="F45" s="1">
         <v>12.039949999999999</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="3">
         <v>12.36969</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45" s="1">
+        <f t="shared" si="12"/>
+        <v>0.43670399999999998</v>
+      </c>
+      <c r="J45" s="3">
+        <f t="shared" si="7"/>
+        <v>0.44580320000000001</v>
+      </c>
+      <c r="K45" s="1">
+        <f t="shared" si="8"/>
+        <v>0.46814800000000001</v>
+      </c>
+      <c r="L45" s="3">
+        <f t="shared" si="9"/>
+        <v>0.48067880000000002</v>
+      </c>
+      <c r="M45" s="1">
+        <f t="shared" si="10"/>
+        <v>0.48159799999999997</v>
+      </c>
+      <c r="N45" s="3">
+        <f t="shared" si="11"/>
+        <v>0.49478759999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>26</v>
       </c>
       <c r="B46" s="1">
         <v>11.01993</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C46" s="3">
         <v>11.32633</v>
       </c>
       <c r="D46" s="1">
         <v>11.833640000000001</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="3">
         <v>12.11576</v>
       </c>
       <c r="F46" s="1">
         <v>12.1723</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="3">
         <v>12.527810000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I46" s="1">
+        <f t="shared" si="12"/>
+        <v>0.4407972</v>
+      </c>
+      <c r="J46" s="3">
+        <f t="shared" si="7"/>
+        <v>0.45305320000000004</v>
+      </c>
+      <c r="K46" s="1">
+        <f t="shared" si="8"/>
+        <v>0.47334560000000003</v>
+      </c>
+      <c r="L46" s="3">
+        <f t="shared" si="9"/>
+        <v>0.48463040000000002</v>
+      </c>
+      <c r="M46" s="1">
+        <f t="shared" si="10"/>
+        <v>0.48689199999999999</v>
+      </c>
+      <c r="N46" s="3">
+        <f t="shared" si="11"/>
+        <v>0.50111240000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>27</v>
       </c>
       <c r="B47" s="1">
         <v>11.29795</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="3">
         <v>11.455220000000001</v>
       </c>
       <c r="D47" s="1">
         <v>12.174300000000001</v>
       </c>
-      <c r="E47" s="4">
+      <c r="E47" s="3">
         <v>12.354150000000001</v>
       </c>
       <c r="F47" s="1">
         <v>12.34158</v>
       </c>
-      <c r="G47" s="4">
+      <c r="G47" s="3">
         <v>12.645799999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I47" s="1">
+        <f t="shared" si="12"/>
+        <v>0.45191799999999999</v>
+      </c>
+      <c r="J47" s="3">
+        <f t="shared" si="7"/>
+        <v>0.45820880000000003</v>
+      </c>
+      <c r="K47" s="1">
+        <f t="shared" si="8"/>
+        <v>0.48697200000000002</v>
+      </c>
+      <c r="L47" s="3">
+        <f t="shared" si="9"/>
+        <v>0.49416600000000005</v>
+      </c>
+      <c r="M47" s="1">
+        <f t="shared" si="10"/>
+        <v>0.49366320000000002</v>
+      </c>
+      <c r="N47" s="3">
+        <f t="shared" si="11"/>
+        <v>0.50583199999999995</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>28</v>
       </c>
       <c r="B48" s="1">
         <v>15.73382</v>
       </c>
-      <c r="C48" s="4">
+      <c r="C48" s="3">
         <v>15.92812</v>
       </c>
       <c r="D48" s="1">
         <v>16.109159999999999</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="3">
         <v>15.543810000000001</v>
       </c>
       <c r="F48" s="1">
         <v>15.79932</v>
       </c>
-      <c r="G48" s="4">
+      <c r="G48" s="3">
         <v>16.044740000000001</v>
+      </c>
+      <c r="I48" s="1">
+        <f t="shared" si="12"/>
+        <v>0.62935279999999993</v>
+      </c>
+      <c r="J48" s="3">
+        <f t="shared" si="7"/>
+        <v>0.63712480000000005</v>
+      </c>
+      <c r="K48" s="1">
+        <f t="shared" si="8"/>
+        <v>0.64436640000000001</v>
+      </c>
+      <c r="L48" s="3">
+        <f t="shared" si="9"/>
+        <v>0.62175239999999998</v>
+      </c>
+      <c r="M48" s="1">
+        <f t="shared" si="10"/>
+        <v>0.6319728</v>
+      </c>
+      <c r="N48" s="3">
+        <f t="shared" si="11"/>
+        <v>0.64178960000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>